<commit_message>
Dodanie funkcjolaności liczenia fazy księżyca
</commit_message>
<xml_diff>
--- a/application_zodiak/funkcjolaności_baza.xlsx
+++ b/application_zodiak/funkcjolaności_baza.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ja\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\oksiedz\Documents\C_plus_plus\application_zodiak\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12589E44-1989-448B-9941-F43E17D036BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="18390" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="18390" windowHeight="11025"/>
   </bookViews>
   <sheets>
     <sheet name="Funkcjonalności" sheetId="1" r:id="rId1"/>
@@ -32,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="114">
   <si>
     <t>Lp</t>
   </si>
@@ -379,7 +378,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -508,8 +507,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -520,11 +522,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,45 +804,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.81640625" customWidth="1"/>
-    <col min="3" max="3" width="88.81640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.85546875" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4"/>
-    </row>
-    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="5" t="s">
+      <c r="C1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="9"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="6"/>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
       <c r="B3" s="3" t="s">
         <v>15</v>
       </c>
@@ -851,8 +850,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="6"/>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
@@ -860,8 +859,8 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="7"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -869,20 +868,20 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+    <row r="6" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="9"/>
+      <c r="C6" s="5"/>
       <c r="D6" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="6"/>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="7"/>
       <c r="B7" s="3" t="s">
         <v>22</v>
       </c>
@@ -890,8 +889,8 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="6"/>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="7"/>
       <c r="B8" s="3" t="s">
         <v>24</v>
       </c>
@@ -899,8 +898,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="6"/>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="7"/>
       <c r="B9" s="3" t="s">
         <v>26</v>
       </c>
@@ -908,8 +907,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="6"/>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="7"/>
       <c r="B10" s="3" t="s">
         <v>28</v>
       </c>
@@ -917,8 +916,8 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="6"/>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="7"/>
       <c r="B11" s="3" t="s">
         <v>30</v>
       </c>
@@ -926,8 +925,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="7"/>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="3" t="s">
         <v>32</v>
       </c>
@@ -935,20 +934,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="5" t="s">
+    <row r="13" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="9"/>
+      <c r="C13" s="5"/>
       <c r="D13" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="6"/>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="7"/>
       <c r="B14" s="3" t="s">
         <v>35</v>
       </c>
@@ -956,8 +955,8 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="6"/>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="7"/>
       <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
@@ -965,8 +964,8 @@
         <v>38</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="7"/>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
@@ -974,20 +973,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="5" t="s">
+    <row r="17" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B17" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C17" s="9"/>
+      <c r="C17" s="5"/>
       <c r="D17" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" s="6"/>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" s="7"/>
       <c r="B18" s="3" t="s">
         <v>46</v>
       </c>
@@ -995,8 +994,8 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" s="7"/>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" s="3" t="s">
         <v>42</v>
       </c>
@@ -1004,20 +1003,20 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="5" t="s">
+    <row r="20" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="9"/>
+      <c r="C20" s="5"/>
       <c r="D20" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A21" s="6"/>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A21" s="7"/>
       <c r="B21" s="3" t="s">
         <v>45</v>
       </c>
@@ -1025,8 +1024,8 @@
         <v>47</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A22" s="6"/>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="7"/>
       <c r="B22" s="3" t="s">
         <v>48</v>
       </c>
@@ -1034,8 +1033,8 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A23" s="6"/>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
       <c r="B23" s="3" t="s">
         <v>49</v>
       </c>
@@ -1043,8 +1042,8 @@
         <v>51</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A24" s="6"/>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
       <c r="B24" s="3" t="s">
         <v>52</v>
       </c>
@@ -1052,244 +1051,134 @@
         <v>53</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A25" s="6"/>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="7"/>
       <c r="B25" s="3" t="s">
         <v>54</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I25">
-        <v>1</v>
-      </c>
-      <c r="J25">
-        <v>0.69020115664821069</v>
-      </c>
-      <c r="K25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A26" s="7"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
       <c r="B26" s="3" t="s">
         <v>62</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I26">
-        <f>1+I25</f>
-        <v>2</v>
-      </c>
-      <c r="J26">
-        <v>0.2859647563937957</v>
-      </c>
-      <c r="K26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="5" t="s">
+    </row>
+    <row r="27" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C27" s="9"/>
+      <c r="C27" s="5"/>
       <c r="D27" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I27">
-        <f t="shared" ref="I27:I36" si="0">1+I26</f>
-        <v>3</v>
-      </c>
-      <c r="J27">
-        <v>0.46033763676657247</v>
-      </c>
-      <c r="K27" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A28" s="6"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" s="7"/>
       <c r="B28" s="3" t="s">
         <v>57</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I28">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="J28">
-        <v>0.82829172773977211</v>
-      </c>
-      <c r="K28" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A29" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="7"/>
       <c r="B29" s="3" t="s">
         <v>59</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I29">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="J29">
-        <v>0.61660311466467765</v>
-      </c>
-      <c r="K29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A30" s="7"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" s="3" t="s">
         <v>61</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I30">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="J30">
-        <v>0.22150344921571796</v>
-      </c>
-      <c r="K30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="5" t="s">
+    </row>
+    <row r="31" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="C31" s="9"/>
+      <c r="C31" s="5"/>
       <c r="D31" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I31">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="J31">
-        <v>0.73909620107909912</v>
-      </c>
-      <c r="K31" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A32" s="6"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="7"/>
       <c r="B32" s="3" t="s">
         <v>64</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I32">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="J32">
-        <v>0.21870185369102546</v>
-      </c>
-      <c r="K32" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A33" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="7"/>
       <c r="B33" s="3" t="s">
         <v>66</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I33">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="J33">
-        <v>1.9065240583089227E-2</v>
-      </c>
-      <c r="K33" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A34" s="7"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="8"/>
       <c r="B34" s="3" t="s">
         <v>67</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I34">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="J34">
-        <v>0.579093498746302</v>
-      </c>
-      <c r="K34" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="5" t="s">
+    </row>
+    <row r="35" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="B35" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="C35" s="9"/>
+      <c r="C35" s="5"/>
       <c r="D35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I35">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="J35">
-        <v>0.42916550784812924</v>
-      </c>
-      <c r="K35" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A36" s="6"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="7"/>
       <c r="B36" s="3" t="s">
         <v>69</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="I36">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="J36">
-        <v>0.57449923995569185</v>
-      </c>
-      <c r="K36" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A37" s="6"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="7"/>
       <c r="B37" s="3" t="s">
         <v>71</v>
       </c>
@@ -1297,21 +1186,21 @@
         <v>104</v>
       </c>
     </row>
-    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="5" t="s">
+    <row r="38" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="8" t="s">
+      <c r="B38" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="5"/>
       <c r="D38" s="1" t="s">
         <v>113</v>
       </c>
       <c r="I38"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A39" s="6"/>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" s="7"/>
       <c r="B39" s="3" t="s">
         <v>73</v>
       </c>
@@ -1319,8 +1208,8 @@
         <v>58</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A40" s="6"/>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" s="7"/>
       <c r="B40" s="3" t="s">
         <v>74</v>
       </c>
@@ -1328,8 +1217,8 @@
         <v>75</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A41" s="6"/>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" s="7"/>
       <c r="B41" s="3" t="s">
         <v>76</v>
       </c>
@@ -1337,8 +1226,8 @@
         <v>77</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A42" s="7"/>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A42" s="8"/>
       <c r="B42" s="3" t="s">
         <v>78</v>
       </c>
@@ -1346,20 +1235,20 @@
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="5" t="s">
+    <row r="43" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="B43" s="8" t="s">
+      <c r="B43" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="C43" s="9"/>
+      <c r="C43" s="5"/>
       <c r="D43" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A44" s="6"/>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A44" s="7"/>
       <c r="B44" s="3" t="s">
         <v>81</v>
       </c>
@@ -1367,8 +1256,8 @@
         <v>82</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A45" s="6"/>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A45" s="7"/>
       <c r="B45" s="3" t="s">
         <v>83</v>
       </c>
@@ -1376,8 +1265,8 @@
         <v>84</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A46" s="6"/>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A46" s="7"/>
       <c r="B46" s="3" t="s">
         <v>85</v>
       </c>
@@ -1385,8 +1274,8 @@
         <v>86</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A47" s="6"/>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A47" s="7"/>
       <c r="B47" s="3" t="s">
         <v>87</v>
       </c>
@@ -1394,8 +1283,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A48" s="7"/>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A48" s="8"/>
       <c r="B48" s="3" t="s">
         <v>89</v>
       </c>
@@ -1403,20 +1292,20 @@
         <v>90</v>
       </c>
     </row>
-    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="5" t="s">
+    <row r="49" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B49" s="8" t="s">
+      <c r="B49" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="C49" s="9"/>
+      <c r="C49" s="5"/>
       <c r="D49" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A50" s="6"/>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="7"/>
       <c r="B50" s="3" t="s">
         <v>91</v>
       </c>
@@ -1424,8 +1313,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="6"/>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
       <c r="B51" s="3" t="s">
         <v>93</v>
       </c>
@@ -1433,8 +1322,8 @@
         <v>94</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="7"/>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
       <c r="B52" s="3" t="s">
         <v>95</v>
       </c>
@@ -1442,20 +1331,20 @@
         <v>96</v>
       </c>
     </row>
-    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="B53" s="8" t="s">
+      <c r="B53" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="9"/>
+      <c r="C53" s="5"/>
       <c r="D53" s="1" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A54" s="6"/>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="7"/>
       <c r="B54" s="3" t="s">
         <v>98</v>
       </c>
@@ -1463,8 +1352,8 @@
         <v>92</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A55" s="6"/>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="7"/>
       <c r="B55" s="3" t="s">
         <v>99</v>
       </c>
@@ -1472,8 +1361,8 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A56" s="6"/>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="7"/>
       <c r="B56" s="3" t="s">
         <v>101</v>
       </c>
@@ -1481,8 +1370,8 @@
         <v>102</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A57" s="7"/>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
       <c r="B57" s="3" t="s">
         <v>103</v>
       </c>
@@ -1492,22 +1381,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B53:C53"/>
-    <mergeCell ref="A49:A52"/>
-    <mergeCell ref="A53:A57"/>
-    <mergeCell ref="A38:A42"/>
-    <mergeCell ref="A43:A48"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A27:A30"/>
-    <mergeCell ref="A31:A34"/>
-    <mergeCell ref="A35:A37"/>
-    <mergeCell ref="B20:C20"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="A2:A5"/>
     <mergeCell ref="A6:A12"/>
@@ -1517,6 +1390,22 @@
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A27:A30"/>
+    <mergeCell ref="A31:A34"/>
+    <mergeCell ref="A35:A37"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B53:C53"/>
+    <mergeCell ref="A49:A52"/>
+    <mergeCell ref="A53:A57"/>
+    <mergeCell ref="A38:A42"/>
+    <mergeCell ref="A43:A48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -1524,23 +1413,23 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>105</v>
       </c>

</xml_diff>